<commit_message>
added functionality to benchmarking tool and improved detection
</commit_message>
<xml_diff>
--- a/out/Analysis/analysis.xlsx
+++ b/out/Analysis/analysis.xlsx
@@ -958,8 +958,6 @@
         <is>
           <t>cmp r3, 0
 moveq r3, 1
-moveq r3, 1
-movne r3, 0
 movne r3, 0</t>
         </is>
       </c>
@@ -1140,19 +1138,6 @@
       <c r="G41" t="b">
         <v>1</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>28, 30</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>.LC0:             .word 2</t>
-        </is>
-      </c>
-      <c r="N41" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
@@ -1172,19 +1157,6 @@
       <c r="G42" t="b">
         <v>1</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>28, 31</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t xml:space="preserve">.LC0:              .word 4 </t>
-        </is>
-      </c>
-      <c r="N42" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
@@ -1204,24 +1176,11 @@
       <c r="G43" t="b">
         <v>1</v>
       </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>28, 32</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>.LC0:             .word 8</t>
-        </is>
-      </c>
-      <c r="N43" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>28-30</t>
+          <t>28, 30</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1236,24 +1195,11 @@
       <c r="G44" t="b">
         <v>1</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>28, 33</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>.LC0:             .word 16</t>
-        </is>
-      </c>
-      <c r="N44" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>28-31</t>
+          <t>28, 31</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1272,7 +1218,7 @@
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>28-32</t>
+          <t>28, 32</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1291,7 +1237,7 @@
     <row r="47">
       <c r="B47" t="inlineStr">
         <is>
-          <t>28-33</t>
+          <t>28, 33</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1369,8 +1315,6 @@
         <is>
           <t>cmp r3, 0
 moveq r3, 1
-moveq r3, 1
-movne r3, 0
 movne r3, 0</t>
         </is>
       </c>
@@ -2148,19 +2092,6 @@
       <c r="G99" t="b">
         <v>1</v>
       </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>30, 32</t>
-        </is>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>.local_arr:     .word 2</t>
-        </is>
-      </c>
-      <c r="N99" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="100">
       <c r="B100" t="inlineStr">
@@ -2180,19 +2111,6 @@
       <c r="G100" t="b">
         <v>1</v>
       </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>30, 33</t>
-        </is>
-      </c>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>.local_arr:               .word 4</t>
-        </is>
-      </c>
-      <c r="N100" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="101">
       <c r="B101" t="inlineStr">
@@ -2212,24 +2130,11 @@
       <c r="G101" t="b">
         <v>1</v>
       </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>30, 34</t>
-        </is>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>.local_arr:       .word 8</t>
-        </is>
-      </c>
-      <c r="N101" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="102">
       <c r="B102" t="inlineStr">
         <is>
-          <t>30-32</t>
+          <t>30, 32</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2244,24 +2149,11 @@
       <c r="G102" t="b">
         <v>1</v>
       </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>30, 35</t>
-        </is>
-      </c>
-      <c r="L102" t="inlineStr">
-        <is>
-          <t xml:space="preserve">.local_arr:       .word 16 </t>
-        </is>
-      </c>
-      <c r="N102" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="103">
       <c r="B103" t="inlineStr">
         <is>
-          <t>30-33</t>
+          <t>30, 33</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2280,7 +2172,7 @@
     <row r="104">
       <c r="B104" t="inlineStr">
         <is>
-          <t>30-34</t>
+          <t>30, 34</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2299,7 +2191,7 @@
     <row r="105">
       <c r="B105" t="inlineStr">
         <is>
-          <t>30-35</t>
+          <t>30, 35</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2768,19 +2660,6 @@
       <c r="G136" t="b">
         <v>1</v>
       </c>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>78-79</t>
-        </is>
-      </c>
-      <c r="L136" t="inlineStr">
-        <is>
-          <t>cmp r3, #1      bne .L5</t>
-        </is>
-      </c>
-      <c r="M136" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="137">
       <c r="B137" t="inlineStr">
@@ -2797,7 +2676,7 @@
       <c r="D137" t="b">
         <v>1</v>
       </c>
-      <c r="H137" t="b">
+      <c r="G137" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3633,7 +3512,7 @@
       <c r="E33" t="b">
         <v>1</v>
       </c>
-      <c r="H33" t="b">
+      <c r="G33" t="b">
         <v>1</v>
       </c>
       <c r="K33" t="inlineStr">
@@ -3664,7 +3543,7 @@
       <c r="E34" t="b">
         <v>1</v>
       </c>
-      <c r="H34" t="b">
+      <c r="G34" t="b">
         <v>1</v>
       </c>
       <c r="K34" t="inlineStr">
@@ -4088,7 +3967,6 @@
         <is>
           <t>cmp r0, 0
 moveq r0, 1
-moveq r0, 1
 beq .L1</t>
         </is>
       </c>
@@ -4109,8 +3987,6 @@
         <is>
           <t>cmp r0, 3
 movgt r0, 0
-movgt r0, 0
-movle r0, 1
 movle r0, 1</t>
         </is>
       </c>
@@ -4226,7 +4102,6 @@
         <is>
           <t>cmp r0, 1
 movne r0, 0
-movne r0, 0
 bne .L16</t>
         </is>
       </c>
@@ -4240,7 +4115,7 @@
     <row r="77">
       <c r="B77" t="inlineStr">
         <is>
-          <t>75-78</t>
+          <t>75, 76, 78</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">

</xml_diff>

<commit_message>
bug fixes and edge cases
</commit_message>
<xml_diff>
--- a/out/Analysis/analysis.xlsx
+++ b/out/Analysis/analysis.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P156"/>
+  <dimension ref="A1:P155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1640,7 +1640,7 @@
       <c r="D72" t="b">
         <v>1</v>
       </c>
-      <c r="H72" t="b">
+      <c r="G72" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2534,398 +2534,397 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129">
-      <c r="B129" t="inlineStr">
+    <row r="129"/>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>harris_constant_simple_insecure</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>17-18</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>num1
+.short 255</t>
+        </is>
+      </c>
+      <c r="E130" t="b">
+        <v>1</v>
+      </c>
+      <c r="G130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>45-46</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>mov r3, 0
+str r3, [fp, #-8]</t>
+        </is>
+      </c>
+      <c r="E131" t="b">
+        <v>1</v>
+      </c>
+      <c r="G131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>47-48</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>mov r3, 1
+str r3, [fp, #-12]</t>
+        </is>
+      </c>
+      <c r="E132" t="b">
+        <v>1</v>
+      </c>
+      <c r="G132" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>49-50</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>mov r3, 4
+str r3, [fp, #-16]</t>
+        </is>
+      </c>
+      <c r="E133" t="b">
+        <v>1</v>
+      </c>
+      <c r="G133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134"/>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>guillermo_compiler_complex_insecure</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>36-37</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>cmp r3, 1
+bne .L2</t>
+        </is>
+      </c>
+      <c r="D135" t="b">
+        <v>1</v>
+      </c>
+      <c r="G135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>77-78</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>cmp r3, 1
+bne .L5</t>
+        </is>
+      </c>
+      <c r="D136" t="b">
+        <v>1</v>
+      </c>
+      <c r="G136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137"/>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>harris_branch_insecure_struct_example</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>46-47</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>cmp r3, 0
+beq .L2</t>
+        </is>
+      </c>
+      <c r="D138" t="b">
+        <v>1</v>
+      </c>
+      <c r="G138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>49-50</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>cmp r3, 1
+bne .L2</t>
+        </is>
+      </c>
+      <c r="D139" t="b">
+        <v>1</v>
+      </c>
+      <c r="G139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>41-42</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>mov r3, 0
+str r3, [fp, #-12]</t>
+        </is>
+      </c>
+      <c r="E140" t="b">
+        <v>1</v>
+      </c>
+      <c r="G140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>43-44</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>mov r3, 1
+str r3, [fp, #-8]</t>
+        </is>
+      </c>
+      <c r="E141" t="b">
+        <v>1</v>
+      </c>
+      <c r="G141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>60-61</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>mov r3, 15
+str r3, [fp, #-16]</t>
+        </is>
+      </c>
+      <c r="E142" t="b">
+        <v>1</v>
+      </c>
+      <c r="G142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143"/>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>harris_branch_simple_insecure</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>38-39</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>cmp r3, 1
+bne .L2</t>
+        </is>
+      </c>
+      <c r="D144" t="b">
+        <v>1</v>
+      </c>
+      <c r="G144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>41-42</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>cmp r3, 1
+bne .L3</t>
+        </is>
+      </c>
+      <c r="D145" t="b">
+        <v>1</v>
+      </c>
+      <c r="G145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>35-36</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>mov r3, 1
+str r3, [fp, #-8]</t>
+        </is>
+      </c>
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
+      <c r="G146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147"/>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>guillermo_loop_simple_insecure</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>63-64</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>cmp r3, 9
+ble .L4</t>
+        </is>
+      </c>
+      <c r="D148" t="b">
+        <v>1</v>
+      </c>
+      <c r="G148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>51-52</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>mov r3, 0
+str r3, [fp, #-8]</t>
+        </is>
+      </c>
+      <c r="E149" t="b">
+        <v>1</v>
+      </c>
+      <c r="G149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="B150" t="inlineStr">
         <is>
           <t>62-64</t>
         </is>
       </c>
-      <c r="C129" t="inlineStr">
+      <c r="C150" t="inlineStr">
         <is>
           <t>ldr r3, [fp, #-8]
 cmp r3, 9
 ble .L4</t>
         </is>
       </c>
-      <c r="F129" t="b">
-        <v>1</v>
-      </c>
-      <c r="H129" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130"/>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>harris_constant_simple_insecure</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>17-18</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>num1
-.short 255</t>
-        </is>
-      </c>
-      <c r="E131" t="b">
-        <v>1</v>
-      </c>
-      <c r="G131" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>45-46</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>mov r3, 0
-str r3, [fp, #-8]</t>
-        </is>
-      </c>
-      <c r="E132" t="b">
-        <v>1</v>
-      </c>
-      <c r="G132" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>47-48</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>mov r3, 1
-str r3, [fp, #-12]</t>
-        </is>
-      </c>
-      <c r="E133" t="b">
-        <v>1</v>
-      </c>
-      <c r="G133" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>49-50</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>mov r3, 4
-str r3, [fp, #-16]</t>
-        </is>
-      </c>
-      <c r="E134" t="b">
-        <v>1</v>
-      </c>
-      <c r="G134" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135"/>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>guillermo_compiler_complex_insecure</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>36-37</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>cmp r3, 1
-bne .L2</t>
-        </is>
-      </c>
-      <c r="D136" t="b">
-        <v>1</v>
-      </c>
-      <c r="G136" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>77-78</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>cmp r3, 1
-bne .L5</t>
-        </is>
-      </c>
-      <c r="D137" t="b">
-        <v>1</v>
-      </c>
-      <c r="G137" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138"/>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>harris_branch_insecure_struct_example</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>46-47</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>cmp r3, 0
-beq .L2</t>
-        </is>
-      </c>
-      <c r="D139" t="b">
-        <v>1</v>
-      </c>
-      <c r="G139" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>49-50</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>cmp r3, 1
-bne .L2</t>
-        </is>
-      </c>
-      <c r="D140" t="b">
-        <v>1</v>
-      </c>
-      <c r="G140" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>41-42</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>mov r3, 0
-str r3, [fp, #-12]</t>
-        </is>
-      </c>
-      <c r="E141" t="b">
-        <v>1</v>
-      </c>
-      <c r="G141" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>43-44</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>mov r3, 1
-str r3, [fp, #-8]</t>
-        </is>
-      </c>
-      <c r="E142" t="b">
-        <v>1</v>
-      </c>
-      <c r="G142" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>60-61</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>mov r3, 15
-str r3, [fp, #-16]</t>
-        </is>
-      </c>
-      <c r="E143" t="b">
-        <v>1</v>
-      </c>
-      <c r="G143" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144"/>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>harris_branch_simple_insecure</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>38-39</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>cmp r3, 1
-bne .L2</t>
-        </is>
-      </c>
-      <c r="D145" t="b">
-        <v>1</v>
-      </c>
-      <c r="G145" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>41-42</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>cmp r3, 1
-bne .L3</t>
-        </is>
-      </c>
-      <c r="D146" t="b">
-        <v>1</v>
-      </c>
-      <c r="G146" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>35-36</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>mov r3, 1
-str r3, [fp, #-8]</t>
-        </is>
-      </c>
-      <c r="E147" t="b">
-        <v>1</v>
-      </c>
-      <c r="G147" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148"/>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>guillermo_loop_simple_insecure</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>63-64</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>cmp r3, 9
-ble .L4</t>
-        </is>
-      </c>
-      <c r="D149" t="b">
-        <v>1</v>
-      </c>
-      <c r="G149" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>51-52</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>mov r3, 0
-str r3, [fp, #-8]</t>
-        </is>
-      </c>
-      <c r="E150" t="b">
+      <c r="F150" t="b">
         <v>1</v>
       </c>
       <c r="G150" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="151">
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>62-64</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>ldr r3, [fp, #-8]
-cmp r3, 9
-ble .L4</t>
-        </is>
-      </c>
-      <c r="F151" t="b">
-        <v>1</v>
-      </c>
-      <c r="G151" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152"/>
-    <row r="153">
-      <c r="A153" t="inlineStr">
+    <row r="151"/>
+    <row r="152">
+      <c r="A152" t="inlineStr">
         <is>
           <t>rpm_plot</t>
         </is>
       </c>
-      <c r="B153" t="inlineStr">
+      <c r="B152" t="inlineStr">
         <is>
           <t>50-51</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
+      <c r="C152" t="inlineStr">
         <is>
           <t>cmp r3, 0
 bne .L2</t>
         </is>
       </c>
+      <c r="D152" t="b">
+        <v>1</v>
+      </c>
+      <c r="G152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>124-125</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>cmp r3, 0
+bne .L6</t>
+        </is>
+      </c>
       <c r="D153" t="b">
         <v>1</v>
       </c>
@@ -2936,13 +2935,13 @@
     <row r="154">
       <c r="B154" t="inlineStr">
         <is>
-          <t>124-125</t>
+          <t>143-144</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>cmp r3, 0
-bne .L6</t>
+          <t>cmp r3, 1
+beq .L8</t>
         </is>
       </c>
       <c r="D154" t="b">
@@ -2955,38 +2954,19 @@
     <row r="155">
       <c r="B155" t="inlineStr">
         <is>
-          <t>143-144</t>
+          <t>153-154</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
-        <is>
-          <t>cmp r3, 1
-beq .L8</t>
-        </is>
-      </c>
-      <c r="D155" t="b">
-        <v>1</v>
-      </c>
-      <c r="G155" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>153-154</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
         <is>
           <t>cmp r3, 81
 beq .L9</t>
         </is>
       </c>
-      <c r="D156" t="b">
-        <v>1</v>
-      </c>
-      <c r="H156" t="b">
+      <c r="D155" t="b">
+        <v>1</v>
+      </c>
+      <c r="H155" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3005,7 +2985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P96"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3110,12 +3090,13 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>25-26</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>cmp r3, 0</t>
+          <t>cmp r3, 0
+bxeq lr</t>
         </is>
       </c>
       <c r="D3" t="b">
@@ -3314,165 +3295,133 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>35-36</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>.word 1</t>
+          <t>local_arr
+.word 1</t>
         </is>
       </c>
       <c r="E21" t="b">
         <v>1</v>
       </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>47-48</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>global_var:         .word 255</t>
-        </is>
-      </c>
-      <c r="N21" t="b">
+      <c r="G21" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>35, 37</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>.word 2</t>
+          <t>local_arr
+.word 2</t>
         </is>
       </c>
       <c r="E22" t="b">
         <v>1</v>
       </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>43-44</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>local_var:         .word 15</t>
-        </is>
-      </c>
-      <c r="N22" t="b">
+      <c r="G22" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>35, 38</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>.word 4</t>
+          <t>local_arr
+.word 4</t>
         </is>
       </c>
       <c r="E23" t="b">
         <v>1</v>
       </c>
-      <c r="H23" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>35-40</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>.local_arr:            .word 1       .word 2       .word 4       .word 8       .word 16</t>
-        </is>
-      </c>
-      <c r="N23" t="b">
+      <c r="G23" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>35, 39</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>.word 8</t>
+          <t>local_arr
+.word 8</t>
         </is>
       </c>
       <c r="E24" t="b">
         <v>1</v>
       </c>
-      <c r="H24" t="b">
+      <c r="G24" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>35, 40</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>.word 16</t>
+          <t>local_arr
+.word 16</t>
         </is>
       </c>
       <c r="E25" t="b">
         <v>1</v>
       </c>
-      <c r="H25" t="b">
+      <c r="G25" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>43-44</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>.word 15</t>
+          <t>local_var
+.word 15</t>
         </is>
       </c>
       <c r="E26" t="b">
         <v>1</v>
       </c>
-      <c r="H26" t="b">
+      <c r="G26" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>47-48</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>.word 255</t>
+          <t>global_var
+.word 255</t>
         </is>
       </c>
       <c r="E27" t="b">
         <v>1</v>
       </c>
-      <c r="H27" t="b">
+      <c r="G27" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3501,12 +3450,13 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>71-72</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>.word 1</t>
+          <t>global_insecure
+.word 1</t>
         </is>
       </c>
       <c r="E33" t="b">
@@ -3517,12 +3467,12 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>75-76</t>
+          <t>51</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>global_secure:         .word 255</t>
+          <t>mov	r0, #16</t>
         </is>
       </c>
       <c r="N33" t="b">
@@ -3532,12 +3482,13 @@
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>75-76</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>.word 255</t>
+          <t>global_secure
+.word 255</t>
         </is>
       </c>
       <c r="E34" t="b">
@@ -3546,297 +3497,288 @@
       <c r="G34" t="b">
         <v>1</v>
       </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>71-72</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>global_insecure: .word 1</t>
-        </is>
-      </c>
-      <c r="N34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>mov	r0, #16</t>
-        </is>
-      </c>
-      <c r="N35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36"/>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+    </row>
+    <row r="35"/>
+    <row r="36">
+      <c r="A36" t="inlineStr">
         <is>
           <t>harris_branch_complex_insecure</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B36" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>cmp r0, 1</t>
         </is>
       </c>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38"/>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37"/>
+    <row r="38">
+      <c r="A38" t="inlineStr">
         <is>
           <t>guillermo_constant_simple_insecure</t>
         </is>
       </c>
     </row>
-    <row r="40"/>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+    <row r="39"/>
+    <row r="40">
+      <c r="A40" t="inlineStr">
         <is>
           <t>guillermo_loop_simple_secure</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>50-51</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>cmp r4, 10
 bne .L3</t>
         </is>
       </c>
-      <c r="D41" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41" t="b">
-        <v>1</v>
-      </c>
-      <c r="K41" t="inlineStr">
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>43, 50-51</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
+      <c r="L40" t="inlineStr">
         <is>
           <t>mov r4, #0       cmp r4, #10     bne .L3</t>
         </is>
       </c>
-      <c r="O41" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42"/>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="O40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41"/>
+    <row r="42">
+      <c r="A42" t="inlineStr">
         <is>
           <t>harris_branch_complex_secure</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>31-32</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>mov r3, 13
 str r3, [sp, #4]</t>
         </is>
       </c>
-      <c r="E43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="inlineStr">
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
         <is>
           <t>33-34</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>mov r3, 192
 str r3, [sp]</t>
         </is>
       </c>
-      <c r="E44" t="b">
-        <v>1</v>
-      </c>
-      <c r="G44" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45"/>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44"/>
+    <row r="45">
+      <c r="A45" t="inlineStr">
         <is>
           <t>harris_branch_insecure_struct_example</t>
         </is>
       </c>
     </row>
-    <row r="47"/>
-    <row r="48">
-      <c r="A48" t="inlineStr">
+    <row r="46"/>
+    <row r="47">
+      <c r="A47" t="inlineStr">
         <is>
           <t>guillermo_branch_complex_insecure</t>
         </is>
       </c>
     </row>
-    <row r="49"/>
-    <row r="50">
-      <c r="A50" t="inlineStr">
+    <row r="48"/>
+    <row r="49">
+      <c r="A49" t="inlineStr">
         <is>
           <t>guillermo_compiler_complex_insecure</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>56-57</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>cmp r0, 1
 bne .L3</t>
         </is>
       </c>
-      <c r="D50" t="b">
-        <v>1</v>
-      </c>
-      <c r="G50" t="b">
-        <v>1</v>
-      </c>
-      <c r="K50" t="inlineStr">
+      <c r="D49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>28-29</t>
         </is>
       </c>
-      <c r="L50" t="inlineStr">
+      <c r="L49" t="inlineStr">
         <is>
           <t>subs r0, r3, #1 movne r0, #1</t>
         </is>
       </c>
-      <c r="M50" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51"/>
-    <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="M49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50"/>
+    <row r="51">
+      <c r="A51" t="inlineStr">
         <is>
           <t>rate_limiting_brute_force</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>82-83</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>cmp r0, 0
 bne .L11</t>
         </is>
       </c>
-      <c r="D52" t="b">
-        <v>1</v>
-      </c>
-      <c r="G52" t="b">
-        <v>1</v>
-      </c>
+      <c r="D51" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>32-33</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>rsbs r0, r0, #1 movcc r0, #0</t>
+        </is>
+      </c>
+      <c r="M51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
       <c r="K52" t="inlineStr">
         <is>
-          <t>32-33</t>
+          <t>70</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>rsbs r0, r0, #1 movcc r0, #0</t>
-        </is>
-      </c>
-      <c r="M52" t="b">
+          <t>mov r4, #3</t>
+        </is>
+      </c>
+      <c r="N52" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="K53" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>88-89</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>mov r4, #3</t>
-        </is>
-      </c>
-      <c r="N53" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>88-89</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
           <t>subs r4, r4, #1 bne .L8</t>
         </is>
       </c>
-      <c r="M54" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55"/>
-    <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="M53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54"/>
+    <row r="55">
+      <c r="A55" t="inlineStr">
         <is>
           <t>guillermo_branch_complex_secure</t>
         </is>
       </c>
     </row>
-    <row r="57"/>
-    <row r="58">
-      <c r="A58" t="inlineStr">
+    <row r="56"/>
+    <row r="57">
+      <c r="A57" t="inlineStr">
         <is>
           <t>data_integrity_checksum</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>27-28</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>cmp r3, 0
 beq .L4</t>
         </is>
       </c>
+      <c r="D57" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>34-35</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>cmp r3, 0
+bne .L3</t>
+        </is>
+      </c>
       <c r="D58" t="b">
         <v>1</v>
       </c>
@@ -3847,149 +3789,154 @@
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>34-35</t>
+          <t>33-35</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
-        <is>
-          <t>cmp r3, 0
-bne .L3</t>
-        </is>
-      </c>
-      <c r="D59" t="b">
-        <v>1</v>
-      </c>
-      <c r="G59" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>33-35</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
         <is>
           <t>ldrb r3, [r2, #1], @, zero_extendqisi2
 cmp r3, 0
 bne .L3</t>
         </is>
       </c>
-      <c r="F60" t="b">
-        <v>1</v>
-      </c>
-      <c r="G60" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61"/>
-    <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60"/>
+    <row r="61">
+      <c r="A61" t="inlineStr">
         <is>
           <t>harris_branch_secure_struct_example</t>
         </is>
       </c>
     </row>
-    <row r="63"/>
+    <row r="62"/>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>secure_data_wipe</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>25-26</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>cmp r1, 0
+bxeq lr</t>
+        </is>
+      </c>
+      <c r="D63" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>33-34</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>cmp r3, r2       bne .L3</t>
+        </is>
+      </c>
+      <c r="O63" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>secure_data_wipe</t>
-        </is>
-      </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>30, 32</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>cmp r1, 0</t>
-        </is>
-      </c>
-      <c r="D64" t="b">
+          <t>mov r1, 0
+strb r1, [r3, #1]</t>
+        </is>
+      </c>
+      <c r="E64" t="b">
         <v>1</v>
       </c>
       <c r="G64" t="b">
         <v>1</v>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>30,32</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>mov r1, #0 ;    strb r1 [r3, #1]!</t>
-        </is>
-      </c>
-      <c r="N64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>33-34</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>cmp r3, r2       bne .L3</t>
-        </is>
-      </c>
-      <c r="O65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66"/>
-    <row r="67">
-      <c r="A67" t="inlineStr">
+    </row>
+    <row r="65"/>
+    <row r="66">
+      <c r="A66" t="inlineStr">
         <is>
           <t>harris_branch_insecure_pointer_example</t>
         </is>
       </c>
     </row>
-    <row r="68"/>
-    <row r="69">
-      <c r="A69" t="inlineStr">
+    <row r="67"/>
+    <row r="68">
+      <c r="A68" t="inlineStr">
         <is>
           <t>guillermo_practical_pin_check</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B68" t="inlineStr">
         <is>
           <t>40-42</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C68" t="inlineStr">
         <is>
           <t>cmp r0, 0
 moveq r0, 1
 beq .L1</t>
         </is>
       </c>
-      <c r="D69" t="b">
-        <v>1</v>
-      </c>
-      <c r="G69" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" t="inlineStr">
+      <c r="D68" t="b">
+        <v>1</v>
+      </c>
+      <c r="G68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="inlineStr">
         <is>
           <t>46-48</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>cmp r0, 3
 movgt r0, 0
 movle r0, 1</t>
         </is>
       </c>
+      <c r="D69" t="b">
+        <v>1</v>
+      </c>
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>71-72</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>cmp r3, 0
+beq .L8</t>
+        </is>
+      </c>
       <c r="D70" t="b">
         <v>1</v>
       </c>
@@ -4000,13 +3947,13 @@
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>71-72</t>
+          <t>76-77</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>cmp r3, 0
-beq .L8</t>
+          <t>cmp r1, 0
+beq .L15</t>
         </is>
       </c>
       <c r="D71" t="b">
@@ -4019,13 +3966,13 @@
     <row r="72">
       <c r="B72" t="inlineStr">
         <is>
-          <t>76-77</t>
+          <t>82-83</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>cmp r1, 0
-beq .L15</t>
+          <t>cmp r3, 0
+bne .L9</t>
         </is>
       </c>
       <c r="D72" t="b">
@@ -4038,13 +3985,13 @@
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>82-83</t>
+          <t>122-123</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>cmp r3, 0
-bne .L9</t>
+          <t>cmp r0, 1
+beq .L23</t>
         </is>
       </c>
       <c r="D73" t="b">
@@ -4057,13 +4004,13 @@
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>122-123</t>
+          <t>127-128</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>cmp r0, 1
-beq .L23</t>
+          <t>cmp r0, 4
+ble .L24</t>
         </is>
       </c>
       <c r="D74" t="b">
@@ -4076,208 +4023,194 @@
     <row r="75">
       <c r="B75" t="inlineStr">
         <is>
-          <t>127-128</t>
+          <t>132-134</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
-        <is>
-          <t>cmp r0, 4
-ble .L24</t>
-        </is>
-      </c>
-      <c r="D75" t="b">
-        <v>1</v>
-      </c>
-      <c r="G75" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>132-134</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
         <is>
           <t>cmp r0, 1
 movne r0, 0
 bne .L16</t>
         </is>
       </c>
-      <c r="D76" t="b">
-        <v>1</v>
-      </c>
-      <c r="G76" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>75, 76, 78</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>ldrb r1, [r2],, 1, @, zero_extendqisi2
-cmp r1, 0
-cmp r1, r3</t>
-        </is>
-      </c>
-      <c r="F77" t="b">
-        <v>1</v>
-      </c>
-      <c r="H77" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" t="inlineStr">
+      <c r="D75" t="b">
+        <v>1</v>
+      </c>
+      <c r="G75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="inlineStr">
         <is>
           <t>81-83</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="C76" t="inlineStr">
         <is>
           <t>ldrb r3, [r0, #1], @, zero_extendqisi2
 cmp r3, 0
 bne .L9</t>
         </is>
       </c>
-      <c r="F78" t="b">
-        <v>1</v>
-      </c>
-      <c r="G78" t="b">
-        <v>1</v>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+      <c r="G76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77"/>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>harris_branch_secure_pointer_example</t>
+        </is>
       </c>
     </row>
     <row r="79"/>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>harris_branch_secure_pointer_example</t>
-        </is>
+          <t>simple_password_check</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>cmp r0, 0</t>
+        </is>
+      </c>
+      <c r="D80" t="b">
+        <v>1</v>
+      </c>
+      <c r="G80" t="b">
+        <v>1</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>32-33</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>rsbs r0, r0, #1 movcc r0, #0</t>
+        </is>
+      </c>
+      <c r="M80" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="81"/>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>simple_password_check</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>cmp r0, 0</t>
-        </is>
-      </c>
-      <c r="D82" t="b">
-        <v>1</v>
-      </c>
-      <c r="G82" t="b">
-        <v>1</v>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>32-33</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>rsbs r0, r0, #1 movcc r0, #0</t>
-        </is>
-      </c>
-      <c r="M82" t="b">
-        <v>1</v>
+          <t>harris_constant_simple_insecure</t>
+        </is>
       </c>
     </row>
     <row r="83"/>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>harris_constant_simple_insecure</t>
-        </is>
-      </c>
-    </row>
-    <row r="85"/>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
           <t>rpm_plot</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="B84" t="inlineStr">
         <is>
           <t>115-116</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C84" t="inlineStr">
         <is>
           <t>cmp r0, 0
 beq .L16</t>
         </is>
       </c>
-      <c r="D86" t="b">
-        <v>1</v>
-      </c>
-      <c r="G86" t="b">
-        <v>1</v>
-      </c>
-      <c r="K86" t="inlineStr">
+      <c r="D84" t="b">
+        <v>1</v>
+      </c>
+      <c r="G84" t="b">
+        <v>1</v>
+      </c>
+      <c r="K84" t="inlineStr">
         <is>
           <t>47-48</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr">
+      <c r="L84" t="inlineStr">
         <is>
           <t>subs r8, r0, #0 beq .L4</t>
         </is>
       </c>
-      <c r="M86" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="B87" t="inlineStr">
+      <c r="M84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="inlineStr">
         <is>
           <t>129-130</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C85" t="inlineStr">
         <is>
           <t>cmp r0, 1
 beq .L11</t>
         </is>
       </c>
-      <c r="D87" t="b">
-        <v>1</v>
-      </c>
-      <c r="G87" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="B88" t="inlineStr">
+      <c r="D85" t="b">
+        <v>1</v>
+      </c>
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="inlineStr">
         <is>
           <t>136-137</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="C86" t="inlineStr">
         <is>
           <t>cmp r3, 81
 bne .L17</t>
         </is>
       </c>
-      <c r="D88" t="b">
-        <v>1</v>
-      </c>
-      <c r="H88" t="b">
+      <c r="D86" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87"/>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>guillermo_compiler_simple_insecure</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>25-26</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>mov r3, 1
+str r3, [r0]</t>
+        </is>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="G88" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4285,95 +4218,71 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>guillermo_compiler_simple_insecure</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>25-26</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>mov r3, 1
-str r3, [r0]</t>
-        </is>
-      </c>
-      <c r="E90" t="b">
-        <v>1</v>
-      </c>
-      <c r="G90" t="b">
-        <v>1</v>
+          <t>guillermo_compiler_simple_secure</t>
+        </is>
       </c>
     </row>
     <row r="91"/>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>guillermo_compiler_simple_secure</t>
-        </is>
-      </c>
-    </row>
-    <row r="93"/>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
           <t>data_encryption_xor</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>cmp r3, 0</t>
-        </is>
-      </c>
-      <c r="D94" t="b">
-        <v>1</v>
-      </c>
-      <c r="G94" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="B95" t="inlineStr">
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>26-27</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>cmp r3, 0
+bxeq lr</t>
+        </is>
+      </c>
+      <c r="D92" t="b">
+        <v>1</v>
+      </c>
+      <c r="G92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="inlineStr">
         <is>
           <t>32-33</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t>cmp r3, 0
 bne .L3</t>
         </is>
       </c>
-      <c r="D95" t="b">
-        <v>1</v>
-      </c>
-      <c r="G95" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="B96" t="inlineStr">
+      <c r="D93" t="b">
+        <v>1</v>
+      </c>
+      <c r="G93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="inlineStr">
         <is>
           <t>31-33</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
+      <c r="C94" t="inlineStr">
         <is>
           <t>ldrb r3, [r0, #1], @, zero_extendqisi2
 cmp r3, 0
 bne .L3</t>
         </is>
       </c>
-      <c r="F96" t="b">
-        <v>1</v>
-      </c>
-      <c r="G96" t="b">
+      <c r="F94" t="b">
+        <v>1</v>
+      </c>
+      <c r="G94" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>